<commit_message>
Entregas Maquina de café movidas a cursos
</commit_message>
<xml_diff>
--- a/Cursos/2021/AI2021_Calificaciones.xlsx
+++ b/Cursos/2021/AI2021_Calificaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pruebasaluuclm-my.sharepoint.com/personal/guillermo_rubiogomez_uclm_es/Documents/UCLM_DOC/09_Docencia/01_AutomatizacionIndustrial/Repo_AI/Cursos/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA70C0D-1061-4141-ADEA-68F6AB0FDFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{BDA70C0D-1061-4141-ADEA-68F6AB0FDFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22EB6939-71C4-4EB7-9DF8-D313044205A3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-1140" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calificaciones" sheetId="1" r:id="rId1"/>
@@ -922,19 +922,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q50"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="5.875" customWidth="1"/>
-    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.8984375" customWidth="1"/>
+    <col min="3" max="3" width="14.69921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="12.625" customWidth="1"/>
-    <col min="14" max="14" width="12.625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="12.625" customWidth="1"/>
-    <col min="17" max="17" width="15.625" customWidth="1"/>
+    <col min="5" max="13" width="12.59765625" customWidth="1"/>
+    <col min="14" max="14" width="12.59765625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="12.59765625" customWidth="1"/>
+    <col min="17" max="17" width="15.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="42.75">
+    <row r="4" spans="1:17" ht="41.4">
       <c r="A4" s="11" t="s">
         <v>97</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>8</v>
       </c>
       <c r="I9" s="14">
-        <v>7.1</v>
+        <v>7.4</v>
       </c>
       <c r="J9" s="14">
         <f>PLC!I9</f>
@@ -1298,7 +1298,7 @@
       <c r="M9" s="14"/>
       <c r="N9" s="14">
         <f t="shared" si="0"/>
-        <v>7.4933333333333332</v>
+        <v>7.5733333333333333</v>
       </c>
       <c r="O9" s="14"/>
       <c r="P9" s="14">
@@ -1307,7 +1307,7 @@
       </c>
       <c r="Q9" s="14">
         <f t="shared" si="2"/>
-        <v>2.9973333333333336</v>
+        <v>3.0293333333333337</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1334,7 +1334,7 @@
         <v>8</v>
       </c>
       <c r="I10" s="14">
-        <v>7.1</v>
+        <v>7.4</v>
       </c>
       <c r="J10" s="14">
         <f>PLC!I10</f>
@@ -1345,7 +1345,7 @@
       <c r="M10" s="14"/>
       <c r="N10" s="14">
         <f t="shared" si="0"/>
-        <v>7.4933333333333332</v>
+        <v>7.5733333333333333</v>
       </c>
       <c r="O10" s="14"/>
       <c r="P10" s="14">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="Q10" s="14">
         <f t="shared" si="2"/>
-        <v>2.9973333333333336</v>
+        <v>3.0293333333333337</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1381,7 +1381,7 @@
         <v>8</v>
       </c>
       <c r="I11" s="14">
-        <v>7.1</v>
+        <v>7.4</v>
       </c>
       <c r="J11" s="14">
         <f>PLC!I11</f>
@@ -1392,7 +1392,7 @@
       <c r="M11" s="14"/>
       <c r="N11" s="14">
         <f t="shared" si="0"/>
-        <v>7.4933333333333332</v>
+        <v>7.5733333333333333</v>
       </c>
       <c r="O11" s="14"/>
       <c r="P11" s="14">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="Q11" s="14">
         <f t="shared" si="2"/>
-        <v>2.9973333333333336</v>
+        <v>3.0293333333333337</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1428,7 +1428,7 @@
         <v>8</v>
       </c>
       <c r="I12" s="14">
-        <v>7.1</v>
+        <v>7.4</v>
       </c>
       <c r="J12" s="14">
         <f>PLC!I12</f>
@@ -1439,7 +1439,7 @@
       <c r="M12" s="14"/>
       <c r="N12" s="14">
         <f t="shared" si="0"/>
-        <v>7.4933333333333332</v>
+        <v>7.5733333333333333</v>
       </c>
       <c r="O12" s="14"/>
       <c r="P12" s="14">
@@ -1448,7 +1448,7 @@
       </c>
       <c r="Q12" s="14">
         <f t="shared" si="2"/>
-        <v>2.9973333333333336</v>
+        <v>3.0293333333333337</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -3285,13 +3285,13 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
-    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.09765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="7" max="7" width="15.125" customWidth="1"/>
-    <col min="9" max="9" width="14.25" customWidth="1"/>
+    <col min="7" max="7" width="15.09765625" customWidth="1"/>
+    <col min="9" max="9" width="14.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
@@ -3324,7 +3324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28.5">
+    <row r="4" spans="1:10" ht="27.6">
       <c r="A4" s="11" t="s">
         <v>97</v>
       </c>
@@ -4878,13 +4878,13 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
-    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.09765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="8" width="15.125" customWidth="1"/>
+    <col min="7" max="8" width="15.09765625" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4915,7 +4915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.5">
+    <row r="4" spans="1:9" ht="27.6">
       <c r="A4" s="11" t="s">
         <v>97</v>
       </c>
@@ -6330,12 +6330,12 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="5.875" customWidth="1"/>
-    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.8984375" customWidth="1"/>
+    <col min="3" max="3" width="14.69921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
@@ -6346,7 +6346,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="28.5">
+    <row r="4" spans="1:6" ht="27.6">
       <c r="A4" s="11" t="s">
         <v>97</v>
       </c>
@@ -7379,15 +7379,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E81954-49D0-4912-B3AC-981DFBDC2EEF}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B38" sqref="B38:B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
-    <col min="3" max="3" width="18.75" customWidth="1"/>
+    <col min="3" max="3" width="18.69921875" customWidth="1"/>
     <col min="4" max="4" width="29.5" customWidth="1"/>
-    <col min="6" max="6" width="18.375" customWidth="1"/>
+    <col min="6" max="6" width="18.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -8824,6 +8824,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B18:B21"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B22:B25"/>
@@ -8831,11 +8836,6 @@
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="B34:B37"/>
     <mergeCell ref="B38:B41"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B18:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>